<commit_message>
make sure the new changes works
</commit_message>
<xml_diff>
--- a/server/excel_controller/config/en/cell-style-samples.xlsx
+++ b/server/excel_controller/config/en/cell-style-samples.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\MayRentManagement\server\excel_controller\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\MayRentManagement\server\excel_controller\config\en\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -409,7 +409,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -604,10 +604,10 @@
     <xf numFmtId="0" fontId="20" fillId="35" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="36" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="29" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="29" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="19" fillId="36" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -934,7 +934,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -951,10 +951,10 @@
       <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E1" s="3" t="s">

</xml_diff>